<commit_message>
take out covid gdp
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
+++ b/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\South Korea\eps-southkorea\InputData\ctrl-settings\EoSEUwGDPiR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B14101-E429-43ED-B3AD-A9FA89917753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AA1AFC-3EC7-47A6-80A6-360B36C8ED08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -904,7 +904,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -961,8 +961,8 @@
         <v>12</v>
       </c>
       <c r="B6" s="6">
-        <f>Calculations!D9</f>
-        <v>2.2413793103448274</v>
+        <f>Calculations!C10</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>